<commit_message>
Added new test case: Add Gift Card
</commit_message>
<xml_diff>
--- a/src/test/java/com/nopCommerce/TestData/CampaignsData.xlsx
+++ b/src/test/java/com/nopCommerce/TestData/CampaignsData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\eclipse-workspace\nopCommerce\src\test\java\com\nopCommerce\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Projects\eclipse-workspace\nopCommerce\src\test\java\com\nopCommerce\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D7BA2B-0215-4FC8-BFF7-0B272129D854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDD90A-3AF3-49D7-87C0-59921489776D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Subject</t>
   </si>
@@ -66,24 +66,6 @@
     <t>Vendors</t>
   </si>
   <si>
-    <t>Registered</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Camp4</t>
-  </si>
-  <si>
-    <t>Camp5</t>
-  </si>
-  <si>
-    <t>Camp6</t>
-  </si>
-  <si>
     <t>Nation</t>
   </si>
   <si>
@@ -91,15 +73,6 @@
   </si>
   <si>
     <t>Election</t>
-  </si>
-  <si>
-    <t>Collage</t>
-  </si>
-  <si>
-    <t>Donate</t>
-  </si>
-  <si>
-    <t>Party</t>
   </si>
 </sst>
 </file>
@@ -448,11 +421,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -484,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -501,10 +472,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -518,67 +489,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>